<commit_message>
updated the completed session informations
</commit_message>
<xml_diff>
--- a/sessions_completed.xlsx
+++ b/sessions_completed.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="65">
   <si>
     <t>Date</t>
   </si>
@@ -186,13 +186,46 @@
   </si>
   <si>
     <t>Matplotlib Basics</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Practice and Softskills</t>
+  </si>
+  <si>
+    <t>CURD Operations using Python GUI with MySql DB (mini project)</t>
+  </si>
+  <si>
+    <t>NumPy functions continued</t>
+  </si>
+  <si>
+    <t>EDA Intro, Need of EDA</t>
+  </si>
+  <si>
+    <t>EDA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +264,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -258,7 +297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -281,11 +320,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -304,6 +403,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,86 +719,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="55.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="55.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2">
         <v>45425</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="C2" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D2" s="3">
         <v>0.5</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>13</v>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>13</v>
@@ -671,28 +810,31 @@
       <c r="J2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2">
         <v>45426</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B3" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="C3" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D3" s="3">
         <v>0.5</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>12</v>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>12</v>
@@ -700,31 +842,34 @@
       <c r="H3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>13</v>
+      <c r="I3" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2">
         <v>45427</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B4" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C4" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D4" s="3">
         <v>0.5</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
+      <c r="E4" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>12</v>
@@ -735,31 +880,34 @@
       <c r="H4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>13</v>
+      <c r="I4" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
         <v>45428</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B5" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="C5" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D5" s="3">
         <v>0.5</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>12</v>
+      <c r="E5" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>12</v>
@@ -770,69 +918,75 @@
       <c r="H5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>13</v>
+      <c r="I5" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
         <v>45432</v>
       </c>
-      <c r="B6" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B6" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C6" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D6" s="3">
         <v>0.5</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>13</v>
+      <c r="G6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
         <v>45433</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B7" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="C7" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D7" s="3">
         <v>0.5</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>12</v>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>12</v>
@@ -840,31 +994,34 @@
       <c r="H7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>13</v>
+      <c r="I7" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
         <v>45434</v>
       </c>
-      <c r="B8" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B8" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C8" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D8" s="3">
         <v>0.5</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>12</v>
@@ -875,31 +1032,34 @@
       <c r="H8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>13</v>
+      <c r="I8" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
         <v>45435</v>
       </c>
-      <c r="B9" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B9" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="C9" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>12</v>
@@ -907,8 +1067,8 @@
       <c r="G9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>13</v>
+      <c r="H9" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>13</v>
@@ -916,25 +1076,28 @@
       <c r="J9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
         <v>45439</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B10" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C10" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>12</v>
@@ -945,31 +1108,34 @@
       <c r="H10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>13</v>
+      <c r="I10" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
         <v>45441</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B11" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C11" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>12</v>
@@ -980,31 +1146,34 @@
       <c r="H11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>13</v>
+      <c r="I11" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
         <v>45442</v>
       </c>
-      <c r="B12" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B12" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="C12" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>12</v>
@@ -1015,31 +1184,34 @@
       <c r="H12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="6" t="s">
-        <v>13</v>
+      <c r="I12" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
         <v>45443</v>
       </c>
-      <c r="B13" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B13" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="C13" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>12</v>
@@ -1047,8 +1219,8 @@
       <c r="G13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>13</v>
+      <c r="H13" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>13</v>
@@ -1056,60 +1228,66 @@
       <c r="J13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
         <v>45446</v>
       </c>
-      <c r="B14" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B14" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C14" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>13</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="5" t="s">
-        <v>12</v>
+      <c r="H14" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="4" t="s">
+      <c r="J14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
         <v>45447</v>
       </c>
-      <c r="B15" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B15" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="C15" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>12</v>
@@ -1123,28 +1301,31 @@
       <c r="I15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" s="4" t="s">
+      <c r="J15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
         <v>45448</v>
       </c>
-      <c r="B16" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B16" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C16" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>12</v>
@@ -1155,31 +1336,34 @@
       <c r="H16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="6" t="s">
-        <v>13</v>
+      <c r="I16" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
         <v>45449</v>
       </c>
-      <c r="B17" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B17" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="C17" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>13</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>13</v>
@@ -1190,31 +1374,34 @@
       <c r="H17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17" s="4" t="s">
+      <c r="I17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
         <v>45450</v>
       </c>
-      <c r="B18" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B18" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="C18" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>12</v>
@@ -1225,37 +1412,40 @@
       <c r="H18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>13</v>
+      <c r="I18" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2">
         <v>45453</v>
       </c>
-      <c r="B19" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B19" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C19" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>12</v>
@@ -1263,28 +1453,31 @@
       <c r="I19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K19" s="4" t="s">
+      <c r="J19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
         <v>45454</v>
       </c>
-      <c r="B20" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B20" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="C20" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>13</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>13</v>
@@ -1298,133 +1491,145 @@
       <c r="I20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="4" t="s">
+      <c r="J20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2">
         <v>45456</v>
       </c>
-      <c r="B21" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B21" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="C21" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>13</v>
+      <c r="G21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2">
         <v>45457</v>
       </c>
-      <c r="B22" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B22" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="C22" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>12</v>
+      <c r="G22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" s="4" t="s">
+      <c r="J22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2">
         <v>45460</v>
       </c>
-      <c r="B23" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B23" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C23" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>13</v>
+      <c r="G23" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K23" s="4" t="s">
+      <c r="I23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2">
         <v>45461</v>
       </c>
-      <c r="B24" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B24" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="C24" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>13</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>13</v>
@@ -1441,25 +1646,28 @@
       <c r="J24" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2">
         <v>45462</v>
       </c>
-      <c r="B25" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B25" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C25" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D25" s="3">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>12</v>
+      <c r="E25" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>12</v>
@@ -1476,31 +1684,34 @@
       <c r="J25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2">
         <v>45464</v>
       </c>
-      <c r="B26" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B26" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="C26" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D26" s="3">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>12</v>
+      <c r="E26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>12</v>
@@ -1508,28 +1719,31 @@
       <c r="I26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J26" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K26" s="4" t="s">
+      <c r="J26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L26" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2">
         <v>45467</v>
       </c>
-      <c r="B27" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B27" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C27" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D27" s="3">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>12</v>
+      <c r="E27" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>12</v>
@@ -1543,28 +1757,31 @@
       <c r="I27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K27" s="4" t="s">
+      <c r="J27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2">
         <v>45469</v>
       </c>
-      <c r="B28" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B28" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C28" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D28" s="3">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>12</v>
+      <c r="E28" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>12</v>
@@ -1572,34 +1789,37 @@
       <c r="G28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K28" s="4" t="s">
+      <c r="H28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L28" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="2">
         <v>45471</v>
       </c>
-      <c r="B29" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B29" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="C29" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D29" s="3">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>12</v>
+      <c r="E29" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>12</v>
@@ -1607,34 +1827,37 @@
       <c r="G29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>12</v>
+      <c r="H29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2">
         <v>45474</v>
       </c>
-      <c r="B30" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B30" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C30" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D30" s="3">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>12</v>
+      <c r="E30" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>12</v>
@@ -1651,25 +1874,28 @@
       <c r="J30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="2">
         <v>45476</v>
       </c>
-      <c r="B31" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B31" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C31" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D31" s="3">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>12</v>
+      <c r="E31" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>12</v>
@@ -1686,25 +1912,28 @@
       <c r="J31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L31" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="2">
         <v>45478</v>
       </c>
-      <c r="B32" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B32" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="C32" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D32" s="3">
         <v>0.97916666666666663</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>12</v>
+      <c r="E32" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>12</v>
@@ -1712,34 +1941,37 @@
       <c r="G32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>12</v>
+      <c r="H32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="J32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="2">
         <v>45481</v>
       </c>
-      <c r="B33" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B33" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C33" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>12</v>
@@ -1756,34 +1988,37 @@
       <c r="J33" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="K33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="2">
         <v>45483</v>
       </c>
-      <c r="B34" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B34" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C34" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>13</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H34" s="5" t="s">
-        <v>12</v>
+      <c r="H34" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>12</v>
@@ -1791,34 +2026,37 @@
       <c r="J34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="K34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="2">
         <v>45485</v>
       </c>
-      <c r="B35" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B35" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="C35" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D35" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>12</v>
+      <c r="G35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>12</v>
@@ -1826,25 +2064,28 @@
       <c r="J35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K35" s="7" t="s">
+      <c r="K35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="2">
         <v>45488</v>
       </c>
-      <c r="B36" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B36" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C36" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D36" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>12</v>
@@ -1861,25 +2102,28 @@
       <c r="J36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K36" s="7" t="s">
+      <c r="K36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="2">
         <v>45490</v>
       </c>
-      <c r="B37" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B37" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C37" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D37" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>12</v>
@@ -1887,34 +2131,37 @@
       <c r="G37" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K37" s="7" t="s">
+      <c r="H37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L37" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="2">
         <v>45492</v>
       </c>
-      <c r="B38" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B38" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="C38" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D38" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>12</v>
@@ -1928,34 +2175,37 @@
       <c r="I38" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J38" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K38" s="7" t="s">
+      <c r="J38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L38" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="2">
         <v>45495</v>
       </c>
-      <c r="B39" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B39" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C39" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>12</v>
@@ -1963,37 +2213,40 @@
       <c r="I39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J39" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K39" s="7" t="s">
+      <c r="J39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L39" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="2">
         <v>45497</v>
       </c>
-      <c r="B40" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B40" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C40" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>13</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H40" s="5" t="s">
-        <v>12</v>
+      <c r="H40" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>12</v>
@@ -2001,25 +2254,28 @@
       <c r="J40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K40" s="7" t="s">
+      <c r="K40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L40" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="2">
         <v>45499</v>
       </c>
-      <c r="B41" s="3">
-        <v>0.41666666666666669</v>
+      <c r="B41" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="C41" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>12</v>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>12</v>
@@ -2036,8 +2292,189 @@
       <c r="J41" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K41" s="7" t="s">
+      <c r="K41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L41" s="7" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="10">
+        <v>45502</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D42" s="12">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="15">
+        <v>45504</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="17">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D43" s="17">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J43" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K43" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="L43" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="15">
+        <v>45506</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="17">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D44" s="17">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="J44" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K44" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L44" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="15">
+        <v>45509</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="17">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D45" s="17">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I45" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J45" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K45" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L45" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="15">
+        <v>45511</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="17">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D46" s="17">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J46" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K46" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="L46" s="18" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>